<commit_message>
Export to excelsheet added. If use external source is enabled. the toolbar has a different control. Start point  for import from excel added. (A1, B2, etc)
</commit_message>
<xml_diff>
--- a/TitleBlock_Template_Example.xlsx
+++ b/TitleBlock_Template_Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68d1a23b9a453310/Personal Files/06_Tools ^0 Software/Portable programs/FreeCAD/Macro/Mod/TechDrawTitleBlockUtility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F904D91B-5656-47D2-87A2-0B6CE8088E67}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CFC94AD-53D6-487F-84A0-6D38BD5DC267}"/>
   <bookViews>
     <workbookView xWindow="17085" yWindow="0" windowWidth="34620" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
small tweaks. column D can now be filled with any char. "No" is removed
</commit_message>
<xml_diff>
--- a/TitleBlock_Template_Example.xlsx
+++ b/TitleBlock_Template_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68d1a23b9a453310/Personal Files/06_Tools ^0 Software/Portable programs/FreeCAD/Macro/Mod/TechDrawTitleBlockUtility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CFC94AD-53D6-487F-84A0-6D38BD5DC267}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035EAD55-3A62-4463-A40F-2F2F0667B986}"/>
   <bookViews>
-    <workbookView xWindow="17085" yWindow="0" windowWidth="34620" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,76 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
-  <si>
-    <t>'Property Name</t>
-  </si>
-  <si>
-    <t>'Property Value</t>
-  </si>
-  <si>
-    <t>'Increase, Yes or No?</t>
-  </si>
-  <si>
-    <t>'AUTHOR_NAME</t>
-  </si>
-  <si>
-    <t>'No</t>
-  </si>
-  <si>
-    <t>'Angle_Units</t>
-  </si>
-  <si>
-    <t>'°',</t>
-  </si>
-  <si>
-    <t>'DN</t>
-  </si>
-  <si>
-    <t>'DRAWING_TITLE</t>
-  </si>
-  <si>
-    <t>'FC-DATE</t>
-  </si>
-  <si>
-    <t>'FC-REV</t>
-  </si>
-  <si>
-    <t>'FC-SC</t>
-  </si>
-  <si>
-    <t>'FC-SH</t>
-  </si>
-  <si>
-    <t>'FC-SI</t>
-  </si>
-  <si>
-    <t>'FreeCAD_DRAWING</t>
-  </si>
-  <si>
-    <t>'FreeCAD DRAWING</t>
-  </si>
-  <si>
-    <t>'Length_Units</t>
-  </si>
-  <si>
-    <t>'mm',</t>
-  </si>
-  <si>
-    <t>'Mass_Units</t>
-  </si>
-  <si>
-    <t>'kg',</t>
-  </si>
-  <si>
-    <t>'Number of sheets</t>
-  </si>
-  <si>
-    <t>'PN</t>
-  </si>
-  <si>
-    <t>'SI-1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Example drawing</t>
   </si>
@@ -118,7 +49,64 @@
     <t>Enter your company name</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Increase value?</t>
+  </si>
+  <si>
+    <t>Property Name</t>
+  </si>
+  <si>
+    <t>Property Value</t>
+  </si>
+  <si>
+    <t>AUTHOR_NAME</t>
+  </si>
+  <si>
+    <t>Angle_Units</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>DRAWING_TITLE</t>
+  </si>
+  <si>
+    <t>FC-DATE</t>
+  </si>
+  <si>
+    <t>FC-REV</t>
+  </si>
+  <si>
+    <t>FC-SC</t>
+  </si>
+  <si>
+    <t>FC-SH</t>
+  </si>
+  <si>
+    <t>FC-SI</t>
+  </si>
+  <si>
+    <t>FreeCAD_DRAWING</t>
+  </si>
+  <si>
+    <t>FreeCAD DRAWING</t>
+  </si>
+  <si>
+    <t>Length_Units</t>
+  </si>
+  <si>
+    <t>Mass_Units</t>
+  </si>
+  <si>
+    <t>Number of sheets</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>SI-1</t>
   </si>
 </sst>
 </file>
@@ -209,9 +197,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}" name="Table2" displayName="Table2" ref="A1:D16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D16" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{100AEE8F-C6BB-495B-8E4E-B450A41D3436}" name="'Property Name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{867C217F-13C5-4A58-996B-0EA430B1B391}" name="'Property Value" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A0427E44-4D52-424E-9A9C-A155840D4F9C}" name="'Increase, Yes or No?" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{100AEE8F-C6BB-495B-8E4E-B450A41D3436}" name="Property Name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{867C217F-13C5-4A58-996B-0EA430B1B391}" name="Property Value" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A0427E44-4D52-424E-9A9C-A155840D4F9C}" name="Increase value?" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{080198E5-BBE1-4EA1-9932-64EC77332367}" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -484,7 +472,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,201 +487,162 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:F6"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C16" xr:uid="{F65F2F4E-4E8F-4462-BB86-A430B13C9E6C}">
-      <formula1>"No, Yes"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Messabox changed to FreeCAD style. Excel will be imported with data only. Formulas are converted to text.
</commit_message>
<xml_diff>
--- a/TitleBlock_Template_Example.xlsx
+++ b/TitleBlock_Template_Example.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68d1a23b9a453310/Personal Files/06_Tools ^0 Software/Portable programs/FreeCAD/Macro/Mod/TechDrawTitleBlockUtility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{035EAD55-3A62-4463-A40F-2F2F0667B986}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46433AF5-6ACC-45BB-8647-3B541EC5CD37}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Example drawing</t>
   </si>
@@ -107,6 +118,12 @@
   </si>
   <si>
     <t>SI-1</t>
+  </si>
+  <si>
+    <t>Paul Ebbers</t>
+  </si>
+  <si>
+    <t>210-05</t>
   </si>
 </sst>
 </file>
@@ -142,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -150,8 +167,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,13 +495,13 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
     <col min="5" max="5" width="1.7109375" customWidth="1"/>
@@ -498,7 +521,7 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -506,12 +529,14 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -520,16 +545,18 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -542,16 +569,19 @@
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45220</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="1"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
a multiplier added to increase number with 10 for example
</commit_message>
<xml_diff>
--- a/TitleBlock_Template_Example.xlsx
+++ b/TitleBlock_Template_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68d1a23b9a453310/Personal Files/06_Tools ^0 Software/Portable programs/FreeCAD/Macro/Mod/TechDrawTitleBlockUtility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46433AF5-6ACC-45BB-8647-3B541EC5CD37}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBD108DC-DECB-4B99-AF19-CADE1BD279E2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Example drawing</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>210-05</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
   </si>
 </sst>
 </file>
@@ -170,17 +173,20 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -217,13 +223,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}" name="Table2" displayName="Table2" ref="A1:D16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D16" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{100AEE8F-C6BB-495B-8E4E-B450A41D3436}" name="Property Name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{867C217F-13C5-4A58-996B-0EA430B1B391}" name="Property Value" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{A0427E44-4D52-424E-9A9C-A155840D4F9C}" name="Increase value?" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{080198E5-BBE1-4EA1-9932-64EC77332367}" name="Remarks" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}" name="Table2" displayName="Table2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E16" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{100AEE8F-C6BB-495B-8E4E-B450A41D3436}" name="Property Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{867C217F-13C5-4A58-996B-0EA430B1B391}" name="Property Value" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A0427E44-4D52-424E-9A9C-A155840D4F9C}" name="Increase value?" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A4D6C63E-EEED-4F27-B38D-F625D45AA6C1}" name="Multiplier" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{080198E5-BBE1-4EA1-9932-64EC77332367}" name="Remarks" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -492,23 +499,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" customWidth="1"/>
-    <col min="6" max="6" width="105.85546875" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="49" customWidth="1"/>
+    <col min="6" max="6" width="1.7109375" customWidth="1"/>
+    <col min="7" max="7" width="105.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -518,14 +525,17 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -533,21 +543,23 @@
         <v>26</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="1"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -556,9 +568,10 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -566,12 +579,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -579,27 +593,30 @@
         <f ca="1">TODAY()</f>
         <v>45220</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -607,17 +624,21 @@
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -625,53 +646,59 @@
         <v>20</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:F6"/>
+    <mergeCell ref="G1:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
error handling added to savasdialog. Started with export settings to excel workbook
</commit_message>
<xml_diff>
--- a/TitleBlock_Template_Example.xlsx
+++ b/TitleBlock_Template_Example.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68d1a23b9a453310/Personal Files/06_Tools ^0 Software/Portable programs/FreeCAD/Macro/Mod/TechDrawTitleBlockUtility/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBD108DC-DECB-4B99-AF19-CADE1BD279E2}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_CB2E68959940D47557F9D959308F8138AE72DF34" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DC6AEC3-E758-4F5D-AA84-0BAB0956F4CD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Settings" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,9 +34,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
-  <si>
-    <t>Example drawing</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+  <si>
+    <t>Property Name</t>
+  </si>
+  <si>
+    <t>Property Value</t>
+  </si>
+  <si>
+    <t>Increase value?</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -51,60 +58,60 @@
 - In the column "remarks" you can add information for your users. for example instructions.</t>
   </si>
   <si>
+    <t>AUTHOR_NAME</t>
+  </si>
+  <si>
+    <t>Paul Ebbers</t>
+  </si>
+  <si>
     <t>Enter your full name</t>
   </si>
   <si>
+    <t>Angle_Units</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>210-05</t>
+  </si>
+  <si>
+    <t>DRAWING_TITLE</t>
+  </si>
+  <si>
+    <t>Example drawing</t>
+  </si>
+  <si>
     <t>Enter the drawing description</t>
   </si>
   <si>
+    <t>FC-DATE</t>
+  </si>
+  <si>
+    <t>FC-REV</t>
+  </si>
+  <si>
+    <t>FC-SC</t>
+  </si>
+  <si>
+    <t>FC-SH</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>FC-SI</t>
+  </si>
+  <si>
+    <t>FreeCAD_DRAWING</t>
+  </si>
+  <si>
+    <t>FreeCAD DRAWING</t>
+  </si>
+  <si>
     <t>Enter your company name</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Increase value?</t>
-  </si>
-  <si>
-    <t>Property Name</t>
-  </si>
-  <si>
-    <t>Property Value</t>
-  </si>
-  <si>
-    <t>AUTHOR_NAME</t>
-  </si>
-  <si>
-    <t>Angle_Units</t>
-  </si>
-  <si>
-    <t>DN</t>
-  </si>
-  <si>
-    <t>DRAWING_TITLE</t>
-  </si>
-  <si>
-    <t>FC-DATE</t>
-  </si>
-  <si>
-    <t>FC-REV</t>
-  </si>
-  <si>
-    <t>FC-SC</t>
-  </si>
-  <si>
-    <t>FC-SH</t>
-  </si>
-  <si>
-    <t>FC-SI</t>
-  </si>
-  <si>
-    <t>FreeCAD_DRAWING</t>
-  </si>
-  <si>
-    <t>FreeCAD DRAWING</t>
-  </si>
-  <si>
     <t>Length_Units</t>
   </si>
   <si>
@@ -120,13 +127,16 @@
     <t>SI-1</t>
   </si>
   <si>
-    <t>Paul Ebbers</t>
-  </si>
-  <si>
-    <t>210-05</t>
-  </si>
-  <si>
-    <t>Multiplier</t>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Use external source</t>
   </si>
 </sst>
 </file>
@@ -162,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,31 +189,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,19 +229,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}" name="Table2" displayName="Table2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E16" xr:uid="{2D465B18-105C-4787-B8E0-D0EFF88B2D8B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{100AEE8F-C6BB-495B-8E4E-B450A41D3436}" name="Property Name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{867C217F-13C5-4A58-996B-0EA430B1B391}" name="Property Value" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A0427E44-4D52-424E-9A9C-A155840D4F9C}" name="Increase value?" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{A4D6C63E-EEED-4F27-B38D-F625D45AA6C1}" name="Multiplier" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{080198E5-BBE1-4EA1-9932-64EC77332367}" name="Remarks" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Property Name" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Property Value" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Increase value?" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Multiplier" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remarks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -501,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -517,90 +524,90 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="G4" s="5"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5"/>
+        <v>14</v>
+      </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3">
         <f ca="1">TODAY()</f>
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -609,7 +616,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -618,11 +625,11 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1">
         <v>10</v>
@@ -631,7 +638,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -640,20 +647,20 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -662,7 +669,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -671,7 +678,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -680,7 +687,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -689,7 +696,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -701,9 +708,45 @@
     <mergeCell ref="G1:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B2" xr:uid="{00000000-0002-0000-0400-000000000000}">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>